<commit_message>
branding manager and configs setup with localization overrides
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization.xlsx
+++ b/Assets/Editor/Localization.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\resource-force\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C3A2527-CFB8-4BDA-8F25-CE73B6C066A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB150A20-4E99-406D-8095-04A854078490}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="StringLocalizations_BasicText" sheetId="8" r:id="rId1"/>
+    <sheet name="Localization" sheetId="8" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="628">
   <si>
     <t>key</t>
   </si>
@@ -1903,6 +1903,12 @@
   </si>
   <si>
     <t>nl</t>
+  </si>
+  <si>
+    <t>BRANDING_FORCE_NAME</t>
+  </si>
+  <si>
+    <t>BRANDING_FORCE_STRAPLINE</t>
   </si>
 </sst>
 </file>
@@ -2304,10 +2310,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4581,6 +4587,16 @@
         <v>616</v>
       </c>
     </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" s="3" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" s="3" t="s">
+        <v>627</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Setup a branding config for inspect rename use manager to use branding objects Start changing the behaviour of language/location selection to be entirely config driven
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization.xlsx
+++ b/Assets/Editor/Localization.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\resource-force\Assets\Editor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\INSPEC2T\ResourceForce\RF_Game\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB150A20-4E99-406D-8095-04A854078490}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="8" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="633">
   <si>
     <t>key</t>
   </si>
@@ -1909,12 +1908,27 @@
   </si>
   <si>
     <t>BRANDING_FORCE_STRAPLINE</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SELECT_LOCATION</t>
+  </si>
+  <si>
+    <t>Select a location</t>
+  </si>
+  <si>
+    <t>Selecteer een locatie</t>
+  </si>
+  <si>
+    <t>Selecciona una ubicación</t>
+  </si>
+  <si>
+    <t>Επιλέξτε μια τοποθεσία</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2308,12 +2322,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3671,894 +3685,894 @@
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
-        <v>158</v>
+        <v>628</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>159</v>
+        <v>629</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>388</v>
+        <v>630</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>271</v>
+        <v>632</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>322</v>
+        <v>631</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>110</v>
+        <v>388</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>110</v>
+        <v>271</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>110</v>
+        <v>322</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>389</v>
+        <v>112</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>272</v>
+        <v>112</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C85" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D85" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E85" s="6" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="3" t="s">
+    <row r="86" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C86" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D86" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="E86" s="6" t="s">
         <v>412</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>408</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>543</v>
+        <v>407</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D90" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E90" s="6" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="3" t="s">
+    <row r="91" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>403</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>400</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E91" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C93" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D93" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E93" s="6" t="s">
         <v>324</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>22</v>
+        <v>185</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>339</v>
+        <v>391</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>217</v>
+        <v>274</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>186</v>
+        <v>22</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>392</v>
+        <v>339</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>275</v>
+        <v>217</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>189</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>325</v>
+        <v>190</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
-        <v>445</v>
+        <v>191</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>446</v>
+        <v>192</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>449</v>
+        <v>394</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>547</v>
+        <v>325</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>578</v>
+        <v>276</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
-        <v>202</v>
+        <v>448</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>203</v>
+        <v>447</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>203</v>
+        <v>548</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
-        <v>434</v>
+        <v>202</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>435</v>
+        <v>203</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>549</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>505</v>
+        <v>435</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>438</v>
+        <v>505</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C106" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="D105" s="4" t="s">
+      <c r="D106" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="E105" s="6" t="s">
+      <c r="E106" s="6" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="3" t="s">
+    <row r="107" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C107" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D107" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="E106" s="6" t="s">
+      <c r="E107" s="6" t="s">
         <v>554</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>611</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C109" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="D109" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="E108" s="6" t="s">
+      <c r="E109" s="6" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="3" t="s">
+    <row r="110" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C110" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D110" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="E109" s="6" t="s">
+      <c r="E110" s="6" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="3" t="s">
+    <row r="111" spans="1:5" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D111" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="E110" s="6" t="s">
+      <c r="E111" s="6" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>589</v>
-      </c>
-      <c r="E111" s="6" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>467</v>
+        <v>516</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C114" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D114" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="E113" s="6" t="s">
+      <c r="E114" s="6" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="3" t="s">
+    <row r="115" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C115" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D115" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="E114" s="6" t="s">
+      <c r="E115" s="6" t="s">
         <v>561</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C117" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D117" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="E116" s="6" t="s">
+      <c r="E117" s="6" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="3" t="s">
+    <row r="118" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D118" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="E117" s="6" t="s">
+      <c r="E118" s="6" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="3" t="s">
+    <row r="119" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C119" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D119" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="E118" s="6" t="s">
+      <c r="E119" s="6" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="D119" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C121" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D121" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="E120" s="6" t="s">
+      <c r="E121" s="6" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="3" t="s">
+    <row r="122" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C122" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D122" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="E121" s="6" t="s">
+      <c r="E122" s="6" t="s">
         <v>567</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="E122" s="6" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C124" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="D123" s="4" t="s">
+      <c r="D124" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="E123" s="6" t="s">
+      <c r="E124" s="6" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A124" s="3" t="s">
+    <row r="125" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A125" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C125" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="D124" s="4" t="s">
+      <c r="D125" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="E124" s="6" t="s">
+      <c r="E125" s="6" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A125" s="3" t="s">
+    <row r="126" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A126" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="C125" s="4" t="s">
+      <c r="C126" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="D125" s="4" t="s">
+      <c r="D126" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="E125" s="6" t="s">
+      <c r="E126" s="6" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A126" s="3" t="s">
+    <row r="127" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A127" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C127" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="D126" s="4" t="s">
+      <c r="D127" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="E126" s="6" t="s">
+      <c r="E127" s="6" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A127" s="3" t="s">
+    <row r="128" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A128" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="C127" s="4" t="s">
+      <c r="C128" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="D127" s="4" t="s">
+      <c r="D128" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="E127" s="6" t="s">
+      <c r="E128" s="6" t="s">
         <v>573</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A128" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="E128" s="6" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A129" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>494</v>
+        <v>534</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A130" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A131" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C131" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="D130" s="4" t="s">
+      <c r="D131" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="E130" s="6" t="s">
+      <c r="E131" s="6" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A131" s="3" t="s">
+    <row r="132" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A132" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B132" s="3" t="s">
         <v>617</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="E131" s="3" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A132" s="3" t="s">
-        <v>614</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>618</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>616</v>
@@ -4572,10 +4586,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>616</v>
@@ -4589,11 +4603,28 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
-        <v>626</v>
+        <v>615</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" s="3" t="s">
         <v>627</v>
       </c>
     </row>

</xml_diff>